<commit_message>
Object Creation Project: - Fixed bug with network creations
</commit_message>
<xml_diff>
--- a/Checkpoint_Object_Creation/config/Object_Creation-Data.xlsx
+++ b/Checkpoint_Object_Creation/config/Object_Creation-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_Object_Creation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B079D26F-030E-4C6B-8AC9-C8C9CD3B3D26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03F333D-1DCD-43ED-A5E4-9EB5B603676C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
+    <workbookView xWindow="5124" yWindow="1812" windowWidth="15132" windowHeight="7980" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Object Name</t>
   </si>
@@ -34,13 +34,28 @@
   </si>
   <si>
     <t>Object Groups</t>
+  </si>
+  <si>
+    <t>Local_User</t>
+  </si>
+  <si>
+    <t>Net_172.16.0.0_24</t>
+  </si>
+  <si>
+    <t>172.16.0.0/24</t>
+  </si>
+  <si>
+    <t>Net_172.16.0.0_25</t>
+  </si>
+  <si>
+    <t>172.16.0.0/25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +74,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -418,7 +439,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,10 +463,26 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -454,6 +491,7 @@
       <c r="A5" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Object Creation Project: - Assigning to group logic added - Creation and modification to network groups added
</commit_message>
<xml_diff>
--- a/Checkpoint_Object_Creation/config/Object_Creation-Data.xlsx
+++ b/Checkpoint_Object_Creation/config/Object_Creation-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_Object_Creation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03F333D-1DCD-43ED-A5E4-9EB5B603676C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18191E24-BEEB-488B-A188-21DDB45E2E5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5124" yWindow="1812" windowWidth="15132" windowHeight="7980" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Object Name</t>
   </si>
@@ -39,16 +39,25 @@
     <t>Local_User</t>
   </si>
   <si>
-    <t>Net_172.16.0.0_24</t>
-  </si>
-  <si>
-    <t>172.16.0.0/24</t>
-  </si>
-  <si>
-    <t>Net_172.16.0.0_25</t>
-  </si>
-  <si>
-    <t>172.16.0.0/25</t>
+    <t>Host_12.0.0.1</t>
+  </si>
+  <si>
+    <t>12.0.0.1</t>
+  </si>
+  <si>
+    <t>Host_12.0.0.3</t>
+  </si>
+  <si>
+    <t>12.0.0.3</t>
+  </si>
+  <si>
+    <t>Net_15.0.0.0</t>
+  </si>
+  <si>
+    <t>15.0.0.0/24</t>
+  </si>
+  <si>
+    <t>Remote_User</t>
   </si>
 </sst>
 </file>
@@ -439,7 +448,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +494,15 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>

</xml_diff>